<commit_message>
MAJ de la plannif v2
</commit_message>
<xml_diff>
--- a/Admimistatif/PlanningV2.xlsx
+++ b/Admimistatif/PlanningV2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Plannification</t>
   </si>
@@ -90,13 +90,16 @@
   </si>
   <si>
     <t>A 2</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +122,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +163,12 @@
     </fill>
     <fill>
       <patternFill patternType="darkUp"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -206,30 +222,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,7 +574,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,344 +583,419 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>42607</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>42608</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>42611</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>42612</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>42613</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="4">
         <v>42614</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>42615</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>42618</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="4">
         <v>42619</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="4">
         <v>42620</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>42621</v>
       </c>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
     </row>
     <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
       <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
MAJ de la plannif
</commit_message>
<xml_diff>
--- a/Admimistatif/PlanningV2.xlsx
+++ b/Admimistatif/PlanningV2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Plannification</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Scaling</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -232,52 +234,55 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -574,7 +579,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,16 +588,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
@@ -653,349 +658,353 @@
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="E11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
     </row>
     <row r="17" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
     </row>
     <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="12"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="10"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ajout du sprite 'jump.png', l'annimation 'run' ne se fait plus lors d'un saut.
</commit_message>
<xml_diff>
--- a/Admimistatif/PlanningV2.xlsx
+++ b/Admimistatif/PlanningV2.xlsx
@@ -276,16 +276,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -579,7 +579,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H4" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,16 +588,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
@@ -679,7 +679,7 @@
       <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -697,7 +697,7 @@
       <c r="E10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -730,7 +730,7 @@
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="22" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="11"/>

</xml_diff>

<commit_message>
ajout d'un tile de test.
</commit_message>
<xml_diff>
--- a/Admimistatif/PlanningV2.xlsx
+++ b/Admimistatif/PlanningV2.xlsx
@@ -579,7 +579,7 @@
   <dimension ref="B2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H1:H1048576"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +769,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>

</xml_diff>